<commit_message>
further work on Data class
</commit_message>
<xml_diff>
--- a/Resources/certificationDataTest.xlsx
+++ b/Resources/certificationDataTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="340" windowWidth="21880" windowHeight="16160" tabRatio="500"/>
+    <workbookView xWindow="8020" yWindow="0" windowWidth="21880" windowHeight="16160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="requirements" sheetId="1" r:id="rId1"/>
@@ -993,7 +993,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
data type specific behaviors
</commit_message>
<xml_diff>
--- a/Resources/certificationDataTest.xlsx
+++ b/Resources/certificationDataTest.xlsx
@@ -990,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1003,7 +1003,7 @@
     <col min="9" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="164">
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="164">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:12">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:12">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:12">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:12">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:12">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1156,6 +1156,16 @@
         <v>0</v>
       </c>
       <c r="H6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="L7" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="B13" s="11">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished data validation for reqs and offs files
</commit_message>
<xml_diff>
--- a/Resources/certificationDataTest.xlsx
+++ b/Resources/certificationDataTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Level One Referee Course</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>tet</t>
   </si>
 </sst>
 </file>
@@ -282,7 +285,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -324,6 +327,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -993,7 +999,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1060,7 +1066,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" s="9">
         <v>0</v>
@@ -1077,16 +1083,16 @@
       <c r="G3" s="9">
         <v>1</v>
       </c>
-      <c r="H3" s="10">
-        <v>1</v>
+      <c r="H3" s="15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8">
-        <v>1</v>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
@@ -1124,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="9">
-        <v>1</v>
+        <v>5.7</v>
       </c>
       <c r="G5" s="9">
         <v>1</v>
@@ -1178,15 +1184,6 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2:XFD1048576 B501:AY1048576">
-      <formula1>0</formula1>
-      <formula2>1</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:AY500">
-      <formula1>"0,1"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">

</xml_diff>